<commit_message>
Agragar la edad a las tablas de decrementos
</commit_message>
<xml_diff>
--- a/Tablas de decrementos.xlsx
+++ b/Tablas de decrementos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peanuts\Desktop\CA-0401 Matemática actuarial ll\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabat\Desktop\Trabajos\2022\UCR\I Semestre\Mate AC II\Proyecto\Proyecto_mate_lab_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAE748F-875F-4957-B3A0-841A4A94F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B018E7F-D2FE-4549-ADB5-CD677E5B0018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7B717DDD-CB3B-4955-AB34-EEE0FB7144D0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7B717DDD-CB3B-4955-AB34-EEE0FB7144D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Invalidez</t>
   </si>
@@ -421,13 +421,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2057E04B-B556-465B-9220-469BD352681A}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K46"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>27</v>
       </c>
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>28</v>
       </c>
@@ -527,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>29</v>
       </c>
@@ -556,7 +556,7 @@
         <v>1.2102370069066755E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>30</v>
       </c>
@@ -585,7 +585,7 @@
         <v>1.7227612820174421E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>31</v>
       </c>
@@ -614,7 +614,7 @@
         <v>2.9953096524158105E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>32</v>
       </c>
@@ -643,7 +643,7 @@
         <v>4.5270451495185574E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>33</v>
       </c>
@@ -672,7 +672,7 @@
         <v>6.2818274189522616E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>34</v>
       </c>
@@ -701,7 +701,7 @@
         <v>7.8860763300229628E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>35</v>
       </c>
@@ -730,7 +730,7 @@
         <v>9.5363812866541559E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>36</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1.08133051475723E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>37</v>
       </c>
@@ -788,7 +788,7 @@
         <v>1.1720299329359769E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>38</v>
       </c>
@@ -817,7 +817,7 @@
         <v>1.240437935561525E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>39</v>
       </c>
@@ -846,7 +846,7 @@
         <v>1.360302253481606E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>40</v>
       </c>
@@ -875,7 +875,7 @@
         <v>1.5565426859351652E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>41</v>
       </c>
@@ -904,7 +904,7 @@
         <v>1.7305362931952844E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>42</v>
       </c>
@@ -933,7 +933,7 @@
         <v>1.7636529942540568E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>43</v>
       </c>
@@ -962,7 +962,7 @@
         <v>1.6384728836954317E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>44</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1.5189018275124895E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>45</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>1.5362092743117987E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>46</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>1.6525514445367925E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>47</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1.7256555727196102E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>48</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>1.6515130172001027E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>49</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>1.4993805756868771E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>50</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>1.3190533850762911E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>51</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>1.1874946017077204E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>52</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>1.0699603614628835E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>53</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>9.886804664103778E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>54</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>9.0746282500436988E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>55</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>8.7235755761035344E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>56</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>9.0070535720523405E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>57</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>9.9958843685468853E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>58</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>1.089734636232734E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>59</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>1.0859299939463092E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>60</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>9.8384870829299311E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>61</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>8.378999849601496E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>62</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>7.4661792743700587E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>63</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>7.2411302376761437E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>64</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>7.4125578346397037E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I42">
         <v>56</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>7.0455479356969111E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I43">
         <v>57</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>5.8709567931391734E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I44">
         <v>58</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>4.2403349401793576E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I45">
         <v>59</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>2.9425067900829433E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I46">
         <v>60</v>
       </c>
@@ -1499,26 +1499,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075F860E-DBC4-437B-AFC9-B89937A9ACAB}">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B117"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1528,10 +1531,13 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1539,10 +1545,13 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1550,10 +1559,13 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1561,10 +1573,13 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1572,10 +1587,13 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1583,10 +1601,13 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1594,10 +1615,13 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1605,10 +1629,13 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1616,10 +1643,13 @@
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1627,10 +1657,13 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1638,10 +1671,13 @@
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1649,10 +1685,13 @@
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1660,10 +1699,13 @@
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1671,10 +1713,13 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1682,10 +1727,13 @@
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1693,10 +1741,13 @@
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1704,10 +1755,13 @@
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1715,10 +1769,13 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1726,10 +1783,13 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1737,494 +1797,629 @@
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>1.3825804973509796E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
         <v>1.3786560221565351E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <v>1.4660001432229731E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>1.4789756072789689E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
         <v>1.5215255321585567E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <v>1.5401954003648177E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
         <v>1.729075154696768E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>1.8627251287316781E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>1.879953473829996E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>1.7254225910593563E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>1.6651461400473385E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>1.7563809355715591E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>1.9908993654574251E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
         <v>1.1174650586757737E-4</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
       <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>2.1537666779421747E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
         <v>1.3174800692139171E-4</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
       <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>2.1262679770627595E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
         <v>1.7634215313255073E-4</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
       <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <v>1.902064769476579E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
         <v>2.3225519468554425E-4</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
       <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <v>1.6056831372337885E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
         <v>2.6885685995609748E-4</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
       <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>1.4065360265946428E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
         <v>2.9292988344947811E-4</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
       <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
         <v>1.3197672243148711E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
         <v>3.18280672310579E-4</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
       <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
         <v>1.428815720640061E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
         <v>4.0450264490731315E-4</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
       <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
         <v>1.5565711078096365E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
         <v>5.2720333823616907E-4</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
       <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
         <v>1.7051101239161247E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
         <v>6.9513037260795964E-4</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
       <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
         <v>1.7938432642479951E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
         <v>8.7577213117045495E-4</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
       <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
         <v>1.9903294742287538E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
         <v>1.128675189346386E-3</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
       <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>2.335253635197424E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
         <v>1.4737665182303818E-3</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
       <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
         <v>2.6161249598590642E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
         <v>1.8929045170676493E-3</v>
       </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
       <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
         <v>2.727437623787602E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
         <v>2.3333725200855074E-3</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
       <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
         <v>2.4896935441413052E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
         <v>2.6941305981624175E-3</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
       <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
         <v>2.1996799805442005E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
         <v>3.0199157778706713E-3</v>
       </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
       <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
         <v>1.88378468651113E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
         <v>3.3082545307205045E-3</v>
       </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
       <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
         <v>1.7325626014625252E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
         <v>3.6565018694150017E-3</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
       <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
         <v>1.638750543754515E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
         <v>3.9855455427661281E-3</v>
       </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
       <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
         <v>1.5535240711345853E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
         <v>4.3306357471550498E-3</v>
       </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
       <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
         <v>1.4168044209628924E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
         <v>4.7739688162300618E-3</v>
       </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
       <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
         <v>1.2633920311155007E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
         <v>5.5022588924536859E-3</v>
       </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
       <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
         <v>1.2425182471454055E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
         <v>6.5815754728778837E-3</v>
       </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
       <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
         <v>1.3961897143391453E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
         <v>7.7690760486460843E-3</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
       <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
         <v>1.5808542791176901E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
         <v>8.6823719269418231E-3</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
       <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
         <v>1.6131851793270485E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
         <v>8.8564939261040997E-3</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
       <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
         <v>1.4425341654024416E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
         <v>8.1101358864989412E-3</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
       <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
         <v>1.3156647475860727E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
         <v>6.619849303926539E-3</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
       <c r="C63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
         <v>5.0486353700878069E-3</v>
       </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
       <c r="C64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
         <v>4.23096001564987E-3</v>
       </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
       <c r="C65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2232,241 +2427,307 @@
       <c r="C66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
         <v>0.46525808712702632</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
         <v>0.3712510888630009</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
         <v>0.33383564783984315</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
         <v>0.33427240900377009</v>
       </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
         <v>0.34309828363245265</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
         <v>0.34043714164301447</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
         <v>0.31689019559568038</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
         <v>0.28209543930820291</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
         <v>0.25172886897749586</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
         <v>0.23376681202325256</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
         <v>0.22265041152536338</v>
       </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
         <v>0.21184926183534267</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
         <v>0.19788304108071311</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
         <v>0.18895043791320776</v>
       </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
         <v>0.17630644169439735</v>
       </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
         <v>0.15559120480617056</v>
       </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
         <v>0.1262978203706544</v>
       </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
         <v>0.14362937872057882</v>
       </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
         <v>0.28106810616631955</v>
       </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
         <v>0.58864881868338126</v>
       </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
         <v>1</v>
       </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -2474,10 +2735,13 @@
       <c r="C88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -2485,10 +2749,13 @@
       <c r="C89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -2496,10 +2763,13 @@
       <c r="C90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -2507,10 +2777,13 @@
       <c r="C91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -2518,10 +2791,13 @@
       <c r="C92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -2529,10 +2805,13 @@
       <c r="C93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -2540,10 +2819,13 @@
       <c r="C94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -2551,10 +2833,13 @@
       <c r="C95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -2562,10 +2847,13 @@
       <c r="C96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -2573,10 +2861,13 @@
       <c r="C97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -2584,10 +2875,13 @@
       <c r="C98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -2595,10 +2889,13 @@
       <c r="C99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -2606,10 +2903,13 @@
       <c r="C100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -2617,10 +2917,13 @@
       <c r="C101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -2628,10 +2931,13 @@
       <c r="C102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -2639,10 +2945,13 @@
       <c r="C103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -2650,10 +2959,13 @@
       <c r="C104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -2661,10 +2973,13 @@
       <c r="C105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -2672,10 +2987,13 @@
       <c r="C106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -2683,10 +3001,13 @@
       <c r="C107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -2694,10 +3015,13 @@
       <c r="C108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -2705,10 +3029,13 @@
       <c r="C109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -2716,10 +3043,13 @@
       <c r="C110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -2727,10 +3057,13 @@
       <c r="C111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -2738,10 +3071,13 @@
       <c r="C112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -2749,10 +3085,13 @@
       <c r="C113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -2760,10 +3099,13 @@
       <c r="C114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -2771,10 +3113,13 @@
       <c r="C115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -2782,15 +3127,21 @@
       <c r="C116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
         <v>0</v>
       </c>
     </row>
@@ -2801,26 +3152,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01479F4B-C493-4EDA-9356-CD3EB25FE9A0}">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2830,10 +3184,13 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2841,10 +3198,13 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2852,10 +3212,13 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2863,10 +3226,13 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2874,10 +3240,13 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2885,10 +3254,13 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2896,10 +3268,13 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2907,10 +3282,13 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2918,10 +3296,13 @@
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2929,10 +3310,13 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2940,10 +3324,13 @@
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2951,10 +3338,13 @@
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2962,10 +3352,13 @@
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2973,10 +3366,13 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2984,10 +3380,13 @@
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2995,10 +3394,13 @@
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3006,10 +3408,13 @@
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3017,10 +3422,13 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3028,10 +3436,13 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3039,648 +3450,825 @@
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>1.2102370069066755E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
         <v>1.7227612820174421E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <v>2.9953096524158105E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>4.5270451495185574E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
         <v>6.2818274189522616E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <v>7.8860763300229628E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
         <v>9.5363812866541559E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>1.08133051475723E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
         <v>2.7461011540206708E-4</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>1.1720299329359769E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
         <v>2.6626267432260743E-4</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
       <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>1.240437935561525E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
         <v>2.4975324541581166E-4</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>1.360302253481606E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
         <v>2.3542760144213849E-4</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
       <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>1.5565426859351652E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
         <v>2.4971535929571586E-4</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
       <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>1.7305362931952844E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
         <v>2.9769526241426729E-4</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
       <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>1.7636529942540568E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
         <v>3.5581587149528077E-4</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
       <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>1.6384728836954317E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
         <v>3.9801603377802455E-4</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
       <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <v>1.5189018275124895E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
         <v>4.3154434117873513E-4</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
       <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <v>1.5362092743117987E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
         <v>4.9974650254838552E-4</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
       <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>1.6525514445367925E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
         <v>6.0416836672878989E-4</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
       <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
         <v>1.7256555727196102E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
         <v>7.2970227167608868E-4</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
       <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
         <v>1.6515130172001027E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
         <v>8.2839327873400806E-4</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
       <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
         <v>1.4993805756868771E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
         <v>9.3984868846707791E-4</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
       <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
         <v>1.3190533850762911E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
         <v>1.0836821396803995E-3</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
       <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
         <v>1.1874946017077204E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
         <v>1.3369048008617472E-3</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
       <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
         <v>1.0699603614628835E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
         <v>1.6699033892998132E-3</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
       <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>9.886804664103778E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
         <v>2.0717047264217697E-3</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
       <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
         <v>9.0746282500436988E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
         <v>2.4673022506791465E-3</v>
       </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
       <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
         <v>8.7235755761035344E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
         <v>2.8776820991616679E-3</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
       <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
         <v>9.0070535720523405E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
         <v>3.343112552348879E-3</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
       <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
         <v>9.9958843685468853E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
         <v>3.9111286120679951E-3</v>
       </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
       <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
         <v>1.089734636232734E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
         <v>4.5494009726479981E-3</v>
       </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
       <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
         <v>1.0859299939463092E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
         <v>5.2241880239926493E-3</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
       <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
         <v>9.8384870829299311E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
         <v>5.9336838703931633E-3</v>
       </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
       <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
         <v>8.378999849601496E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
         <v>6.7880329463534889E-3</v>
       </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
       <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
         <v>7.4661792743700587E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
         <v>7.7618288740580075E-3</v>
       </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
       <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
         <v>7.2411302376761437E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
         <v>8.7678313311365785E-3</v>
       </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
       <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
         <v>7.4125578346397037E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
         <v>9.4239982717641887E-3</v>
       </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
       <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
         <v>7.0455479356969111E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
         <v>9.5064450851203436E-3</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
       <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
         <v>5.8709567931391734E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
         <v>8.8089928786391457E-3</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
       <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
         <v>4.2403349401793576E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
         <v>7.5322772461588298E-3</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
       <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
         <v>2.9425067900829433E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
         <v>5.930285283457782E-3</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
       <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
         <v>2.3891871501514146E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
         <v>4.4218469625577628E-3</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
       <c r="C63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
         <v>3.2648342087967575E-3</v>
       </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
       <c r="C64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
         <v>2.5836869774919996E-3</v>
       </c>
-      <c r="B65">
+      <c r="C65">
         <v>0.68399658672463626</v>
       </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
         <v>2.3332393673920868E-3</v>
       </c>
-      <c r="B66">
+      <c r="C66">
         <v>0.64730637701488525</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
         <v>0.58442674970387287</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
         <v>0.50150559029906971</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
         <v>0.41531186397925357</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
         <v>0.35945590349539319</v>
       </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
         <v>0.34575538205474121</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
         <v>0.38833979773627886</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
         <v>0.44449693335716722</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
         <v>0.4887828824553288</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
         <v>0.4899942853183355</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
         <v>0.50088626495620736</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
         <v>0.57472782900046748</v>
       </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
         <v>0.75883707888848639</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
         <v>1</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -3688,10 +4276,13 @@
       <c r="C80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -3699,10 +4290,13 @@
       <c r="C81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -3710,10 +4304,13 @@
       <c r="C82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -3721,10 +4318,13 @@
       <c r="C83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -3732,10 +4332,13 @@
       <c r="C84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -3743,10 +4346,13 @@
       <c r="C85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -3754,10 +4360,13 @@
       <c r="C86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -3765,10 +4374,13 @@
       <c r="C87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -3776,10 +4388,13 @@
       <c r="C88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -3787,10 +4402,13 @@
       <c r="C89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -3798,10 +4416,13 @@
       <c r="C90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -3809,10 +4430,13 @@
       <c r="C91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -3820,10 +4444,13 @@
       <c r="C92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -3831,10 +4458,13 @@
       <c r="C93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -3842,10 +4472,13 @@
       <c r="C94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -3853,10 +4486,13 @@
       <c r="C95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -3864,10 +4500,13 @@
       <c r="C96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -3875,10 +4514,13 @@
       <c r="C97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -3886,10 +4528,13 @@
       <c r="C98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -3897,10 +4542,13 @@
       <c r="C99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -3908,10 +4556,13 @@
       <c r="C100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -3919,10 +4570,13 @@
       <c r="C101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -3930,10 +4584,13 @@
       <c r="C102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -3941,10 +4598,13 @@
       <c r="C103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -3952,10 +4612,13 @@
       <c r="C104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -3963,10 +4626,13 @@
       <c r="C105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -3974,10 +4640,13 @@
       <c r="C106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -3985,10 +4654,13 @@
       <c r="C107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -3996,10 +4668,13 @@
       <c r="C108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -4007,10 +4682,13 @@
       <c r="C109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -4018,10 +4696,13 @@
       <c r="C110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -4029,10 +4710,13 @@
       <c r="C111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -4040,10 +4724,13 @@
       <c r="C112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -4051,10 +4738,13 @@
       <c r="C113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -4062,10 +4752,13 @@
       <c r="C114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -4073,10 +4766,13 @@
       <c r="C115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -4084,15 +4780,21 @@
       <c r="C116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
         <v>0</v>
       </c>
     </row>

</xml_diff>